<commit_message>
Finished Bill of Materials.
</commit_message>
<xml_diff>
--- a/hardware/BerndoKeyboard-Switchboard/Project Outputs for BerndoKeyboard-Switchboard/BerndoKeyboard-BillOfMaterials.xlsx
+++ b/hardware/BerndoKeyboard-Switchboard/Project Outputs for BerndoKeyboard-Switchboard/BerndoKeyboard-BillOfMaterials.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911509A7-CB87-4A27-A03D-3056A8750885}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B57FB0-D8B6-4C83-8E41-2BED02D5D0EC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,6 +12,7 @@
     <sheet name="BOM" sheetId="2" r:id="rId2"/>
     <sheet name="DigiKey Order List" sheetId="3" r:id="rId3"/>
     <sheet name="LCSC Order List" sheetId="4" r:id="rId4"/>
+    <sheet name="Mouser Order List" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="198">
   <si>
     <t>Comment</t>
   </si>
@@ -584,6 +585,45 @@
   </si>
   <si>
     <t>C77978</t>
+  </si>
+  <si>
+    <t>C7519</t>
+  </si>
+  <si>
+    <t>MOQ: 5 - STEP: 5</t>
+  </si>
+  <si>
+    <t>C114586</t>
+  </si>
+  <si>
+    <t>C60490</t>
+  </si>
+  <si>
+    <t>C114759</t>
+  </si>
+  <si>
+    <t>C105872</t>
+  </si>
+  <si>
+    <t>C163475</t>
+  </si>
+  <si>
+    <t>C327333</t>
+  </si>
+  <si>
+    <t>C128392</t>
+  </si>
+  <si>
+    <t>C7843</t>
+  </si>
+  <si>
+    <t>Mouser</t>
+  </si>
+  <si>
+    <t>621-AP3419KTTR-G1</t>
+  </si>
+  <si>
+    <t>Total BOM Cost / Unit:</t>
   </si>
 </sst>
 </file>
@@ -651,7 +691,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -693,6 +733,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1945,13 +1991,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84E78FC2-A3E1-4959-884F-11794EAA8765}">
-  <dimension ref="A1:Q27"/>
+  <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="I16" sqref="I16"/>
+      <selection pane="bottomRight" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1965,7 +2011,7 @@
     <col min="7" max="7" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="13.28515625" style="10" customWidth="1"/>
-    <col min="11" max="11" width="46.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="46.7109375" style="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="30" style="10" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.42578125" style="10"/>
@@ -2090,7 +2136,6 @@
       <c r="J6" s="10">
         <v>0.27882000000000001</v>
       </c>
-      <c r="K6" s="12"/>
       <c r="P6" s="12"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -2121,7 +2166,6 @@
       <c r="J7" s="10">
         <v>0</v>
       </c>
-      <c r="K7" s="12"/>
       <c r="M7" s="2"/>
       <c r="O7" s="10"/>
       <c r="P7" s="12"/>
@@ -2157,7 +2201,6 @@
       <c r="J8" s="10">
         <v>0.81847999999999999</v>
       </c>
-      <c r="K8" s="12"/>
       <c r="P8" s="12"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -2287,7 +2330,6 @@
       <c r="J11" s="10">
         <v>0.68355999999999995</v>
       </c>
-      <c r="K11" s="12"/>
       <c r="P11" s="12"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -2321,7 +2363,6 @@
       <c r="J12" s="10">
         <v>0.66557999999999995</v>
       </c>
-      <c r="K12" s="12"/>
       <c r="P12" s="12"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -2355,7 +2396,6 @@
       <c r="J13" s="10">
         <v>0.10793</v>
       </c>
-      <c r="K13" s="12"/>
       <c r="P13" s="12"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -2389,7 +2429,6 @@
       <c r="J14" s="10">
         <v>1.24</v>
       </c>
-      <c r="K14" s="12"/>
       <c r="P14" s="12"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -2421,7 +2460,7 @@
         <v>1.1247999999999999E-2</v>
       </c>
       <c r="J15" s="10">
-        <v>0.56000000000000005</v>
+        <v>1.69</v>
       </c>
       <c r="K15" s="12" t="s">
         <v>183</v>
@@ -2459,7 +2498,21 @@
       <c r="F16" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="K16" s="12"/>
+      <c r="G16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="I16" s="10">
+        <v>6.9866999999999999E-2</v>
+      </c>
+      <c r="J16" s="10">
+        <v>0.35</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>186</v>
+      </c>
       <c r="L16" s="2" t="s">
         <v>15</v>
       </c>
@@ -2493,17 +2546,16 @@
       <c r="F17" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K17" s="12"/>
-      <c r="L17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="M17" s="2" t="s">
+      <c r="G17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="N17" s="10">
+      <c r="I17" s="10">
         <v>1.29</v>
       </c>
-      <c r="O17" s="10">
+      <c r="J17" s="10">
         <v>1.29</v>
       </c>
       <c r="P17" s="12"/>
@@ -2527,9 +2579,20 @@
       <c r="F18" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="K18" s="12"/>
-      <c r="L18" s="2" t="s">
+      <c r="G18" s="2" t="s">
         <v>59</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="I18" s="10">
+        <v>9.0108999999999995E-2</v>
+      </c>
+      <c r="J18" s="10">
+        <v>1.35</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>186</v>
       </c>
       <c r="M18" s="2"/>
       <c r="O18" s="10"/>
@@ -2554,17 +2617,16 @@
       <c r="F19" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="K19" s="12"/>
-      <c r="L19" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="M19" s="2" t="s">
+      <c r="G19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="N19" s="10">
+      <c r="I19" s="10">
         <v>1.1000000000000001</v>
       </c>
-      <c r="O19" s="10">
+      <c r="J19" s="10">
         <v>1.1000000000000001</v>
       </c>
       <c r="P19" s="12"/>
@@ -2588,7 +2650,21 @@
       <c r="F20" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="K20" s="12"/>
+      <c r="G20" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="I20" s="10">
+        <v>4.4900000000000002E-4</v>
+      </c>
+      <c r="J20" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="K20" s="12" t="s">
+        <v>182</v>
+      </c>
       <c r="L20" s="2" t="s">
         <v>15</v>
       </c>
@@ -2622,7 +2698,21 @@
       <c r="F21" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="K21" s="12"/>
+      <c r="G21" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="I21" s="10">
+        <v>4.44E-4</v>
+      </c>
+      <c r="J21" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="K21" s="12" t="s">
+        <v>182</v>
+      </c>
       <c r="L21" s="2" t="s">
         <v>15</v>
       </c>
@@ -2656,7 +2746,21 @@
       <c r="F22" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="K22" s="12"/>
+      <c r="G22" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="I22" s="10">
+        <v>4.2700000000000002E-4</v>
+      </c>
+      <c r="J22" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="K22" s="12" t="s">
+        <v>182</v>
+      </c>
       <c r="L22" s="2" t="s">
         <v>15</v>
       </c>
@@ -2690,7 +2794,21 @@
       <c r="F23" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="K23" s="12"/>
+      <c r="G23" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="I23" s="10">
+        <v>9.8200000000000002E-4</v>
+      </c>
+      <c r="J23" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="K23" s="12" t="s">
+        <v>182</v>
+      </c>
       <c r="L23" s="2" t="s">
         <v>15</v>
       </c>
@@ -2724,6 +2842,21 @@
       <c r="F24" s="2" t="s">
         <v>145</v>
       </c>
+      <c r="G24" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="I24" s="10">
+        <v>4.6900000000000002E-4</v>
+      </c>
+      <c r="J24" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="K24" s="12" t="s">
+        <v>182</v>
+      </c>
       <c r="L24" s="2" t="s">
         <v>15</v>
       </c>
@@ -2756,6 +2889,18 @@
       <c r="F25" s="2" t="s">
         <v>163</v>
       </c>
+      <c r="G25" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="I25" s="10">
+        <v>0.74019900000000005</v>
+      </c>
+      <c r="J25" s="10">
+        <v>1.48</v>
+      </c>
       <c r="L25" s="2" t="s">
         <v>15</v>
       </c>
@@ -2788,6 +2933,18 @@
       <c r="F26" s="2" t="s">
         <v>169</v>
       </c>
+      <c r="G26" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="I26" s="10">
+        <v>0.21810599999999999</v>
+      </c>
+      <c r="J26" s="10">
+        <v>0.21810599999999999</v>
+      </c>
       <c r="L26" s="2" t="s">
         <v>15</v>
       </c>
@@ -2820,6 +2977,18 @@
       <c r="F27" s="2" t="s">
         <v>175</v>
       </c>
+      <c r="G27" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="I27" s="10">
+        <v>0.36899999999999999</v>
+      </c>
+      <c r="J27" s="10">
+        <v>0.36899999999999999</v>
+      </c>
       <c r="L27" s="2" t="s">
         <v>15</v>
       </c>
@@ -2827,6 +2996,15 @@
         <v>178</v>
       </c>
       <c r="O27" s="10"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I28" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="J28" s="16">
+        <f>SUM(J6:J27)</f>
+        <v>12.151475999999999</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2834,22 +3012,25 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="C17 A17" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4710C81-D63A-4427-AB96-C9359D37DEC2}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C7"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.7109375" style="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="11.42578125" style="13"/>
   </cols>
   <sheetData>
@@ -2862,6 +3043,94 @@
       </c>
       <c r="C1" s="14" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="13">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="13">
+        <v>7</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="13">
+        <v>1</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="13">
+        <v>1</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="13">
+        <v>1</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="13">
+        <v>1</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="13">
+        <v>1</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="13">
+        <v>1</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -2871,10 +3140,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26A8F462-C2CD-49E1-A3E6-9F6BA1A061E8}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2896,6 +3165,181 @@
         <v>66</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="13">
+        <v>15</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="13">
+        <v>1</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="13">
+        <v>132</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="13">
+        <v>1</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="13">
+        <v>11</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="13">
+        <v>26</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="13">
+        <v>7</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="13">
+        <v>2</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="13">
+        <v>1</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="13">
+        <v>1</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="13">
+        <v>2</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="13">
+        <v>1</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>194</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2A8630B-C072-4B59-8DF5-6B0B1D9C81A8}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="11.42578125" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="13">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>196</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>